<commit_message>
SQL code, allocate course
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\coding\MIS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E54176AD-3092-458D-82E1-29D05C8C9569}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1589447-F70B-400E-A3D1-B9CA6F8A72CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{EDD833FA-799A-4030-8C92-F7D6AA5CAD0D}"/>
   </bookViews>
@@ -39,9 +39,6 @@
     <t>ProgramType</t>
   </si>
   <si>
-    <t>Semester</t>
-  </si>
-  <si>
     <t>CS F213</t>
   </si>
   <si>
@@ -127,6 +124,9 @@
   </si>
   <si>
     <t>WILP</t>
+  </si>
+  <si>
+    <t>SEMESTER</t>
   </si>
 </sst>
 </file>
@@ -591,7 +591,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -617,211 +617,211 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="11" t="s">
-        <v>32</v>
-      </c>
       <c r="E6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="11" t="s">
-        <v>32</v>
-      </c>
       <c r="E12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>